<commit_message>
Update data fields and improve Excel integration
Revised data field names for consistency across ship, weapon, and component data structures. Enhanced Excel update mechanism by integrating openpyxl for better handling of existing workbooks and preserving formatting.
</commit_message>
<xml_diff>
--- a/Abyssal_Ship_Hardware.xlsx
+++ b/Abyssal_Ship_Hardware.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7125" yWindow="3435" windowWidth="33915" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,7 +11,7 @@
     <sheet name="Components" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -28,7 +27,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -48,23 +49,59 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -427,13 +464,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="30.42578125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="8.140625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="11.5703125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="6.42578125" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="11.140625" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="64.7109375" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="15.5703125" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="6.5703125" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="58.85546875" customWidth="1" min="11" max="11"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -478,12 +528,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Ammo Capacity</t>
+          <t>Component Size</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Weight</t>
+          <t>Rating</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -495,29 +545,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hades 5 Missile</t>
+          <t>MRML-3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Medium Range Missile</t>
+          <t>Medium-Range Missile Launcher</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Medium Range</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1d12+8</t>
+          <t>3d8</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -526,124 +576,420 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>High acceleration, explosive payload</t>
+          <t>Lock-on targeting, can be loaded with various missile types.</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="J2" t="n">
+        <v>18</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>A powerful medium-range missile with high accuracy.</t>
+          <t>The MRML-3 is a versatile missile launcher designed for medium-range engagements. It offers lock-on targeting and can be loaded with different types of missiles, making it adaptable to various combat scenarios.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Viper Strike Torpedo</t>
+          <t>PDGW-4</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Torpedo</t>
+          <t>Point Defense Gauss Weapon</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Long, Extreme</t>
+          <t>Short Range</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2d12+8</t>
+          <t>2d6</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Single</t>
+          <t>Rapid Fire</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>High-speed pursuit, advanced evasion algorithms, delayed detonation for critical hits.</t>
+          <t>High rate of fire, effective against incoming projectiles and small craft.</t>
         </is>
       </c>
       <c r="I3" t="n">
         <v>1</v>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Heavy</t>
-        </is>
+      <c r="J3" t="n">
+        <v>15</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>The Viper Strike Torpedo is designed for maximum damage at long ranges. Its advanced evasion systems make it difficult to intercept, and the delayed detonation allows it to penetrate deep into enemy vessels before exploding.</t>
+          <t>The PDGW-4 is a rapid-fire Gauss weapon designed for point defense. It is effective against incoming projectiles, missiles, and small craft, providing an essential layer of defense for the ship.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Inferno Warhead</t>
+          <t>HIL-2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>High Intensity Laser</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Long Range</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3d10</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Sustained</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Capable of cutting through armor, effective against larger vessels.</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>The HIL-2 is a high-intensity laser weapon designed for long-range engagements. It is capable of cutting through heavy armor and is particularly effective against larger vessels.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SMS-1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Short Range Missile</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Close Quarter, Near</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>4d10+12</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Short Range</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2d8</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>8</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Compact size, capable of engaging multiple targets with quick reloading.</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
         <v>14</v>
       </c>
-      <c r="F4" t="n">
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>The SMS-1 is a compact short-range missile system designed for quick and efficient engagements. It delivers 2d8 damage with moderate penetration, making it effective against lightly armored targets or for point defense. The system is designed for rapid reloading, allowing for quick follow-up shots in combat situations.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SMS-1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Short Range Missile</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Short Range</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2d8</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Compact size, capable of engaging multiple targets with quick reloading.</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
         <v>1</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>The SMS-1 is a compact short-range missile system designed for quick and efficient engagements. It delivers 2d8 damage with moderate penetration, making it effective against lightly armored targets or for point defense. The system is designed for rapid reloading, allowing for quick follow-up shots in combat situations.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>LCGC-7</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Large Calibre Gauss Cannon</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Long Range</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>4d10</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" t="n">
+        <v>6</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Sustained</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>High penetration, effective against heavily armored targets and capital ships.</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>The LCGC-7 is a powerful long-range weapon system designed to punch through heavy armor with ease. Capable of dealing massive damage with 4d10 and high penetration, it's ideal for engaging large vessels or fortified structures. Its sustained rate of fire ensures it can maintain pressure on targets over extended engagements.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PDGT-4</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Point Defense Gauss Weapon</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Short Range</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2d6</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Rapid Fire</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>High rate of fire, optimized for intercepting incoming missiles and small craft.</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>The PDGT-4 is a rapid-fire Gauss weapon system designed for point defense. It excels at intercepting incoming missiles, projectiles, and small enemy craft, making it an essential defensive weapon for any ship. Its high rate of fire ensures that threats are neutralized quickly and efficiently.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>HIPL-9</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>High Intensity Laser</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Medium Range</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3d8</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>12</v>
+      </c>
+      <c r="F9" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Burst</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Capable of precise strikes, effective against both shields and armor.</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>The HIPL-9 is a versatile medium-range laser weapon, capable of delivering powerful burst attacks that can penetrate shields and armor alike. Its precision targeting and high damage output make it a formidable choice for both offensive and defensive engagements.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>TLS-12</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Torpedo</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Long Range</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5d12</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>18</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Large explosive payload with high area-of-effect damage.</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2 missiles</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Heavy</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>The Inferno Warhead is a devastating short-range missile designed to deliver a massive explosive payload. Its high penetration and large area-of-effect make it ideal for close-quarters combat, overwhelming enemy defenses and causing significant structural damage.</t>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Heavy damage, capable of delivering devastating blows to large targets.</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>3</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>The TLS-12 is a heavy-duty torpedo launcher system designed for long-range engagements. It delivers devastating damage with 5d12 and very high penetration, making it the perfect weapon for crippling or destroying capital ships and heavily fortified installations. Its single-shot capacity requires careful targeting, but the impact is well worth it.</t>
         </is>
       </c>
     </row>
@@ -658,263 +1004,168 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="23.5703125" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
+    <col width="9.85546875" bestFit="1" customWidth="1" style="9" min="2" max="2"/>
+    <col width="16.28515625" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
+    <col width="12.42578125" customWidth="1" style="9" min="4" max="4"/>
+    <col width="13.85546875" customWidth="1" style="9" min="5" max="5"/>
+    <col width="14.140625" customWidth="1" style="9" min="6" max="6"/>
+    <col width="9.28515625" customWidth="1" style="9" min="7" max="7"/>
+    <col width="6.5703125" bestFit="1" customWidth="1" style="9" min="8" max="8"/>
+    <col width="11" customWidth="1" style="9" min="9" max="9"/>
+    <col width="15.42578125" bestFit="1" customWidth="1" style="9" min="10" max="10"/>
+    <col width="6.42578125" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
+    <col width="27.7109375" customWidth="1" style="6" min="12" max="12"/>
+    <col width="24.28515625" customWidth="1" style="6" min="13" max="13"/>
+    <col width="9.140625" customWidth="1" style="10" min="14" max="15"/>
+    <col width="58" customWidth="1" style="6" min="16" max="16"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="45" customFormat="1" customHeight="1" s="3">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Ship Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>Size (GST)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Acceleration (Cruise/March/Max in Gs)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
+        <is>
+          <t>Component Slots</t>
+        </is>
+      </c>
+      <c r="D1" s="8" t="inlineStr">
+        <is>
+          <t>Acceleration (MaxG)</t>
+        </is>
+      </c>
+      <c r="E1" s="8" t="inlineStr">
         <is>
           <t>Structural Endurance (StE)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="8" t="inlineStr">
         <is>
           <t>Electronic Endurance (ElE)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="8" t="inlineStr">
         <is>
           <t>Signal Rating (SiR)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="8" t="inlineStr">
         <is>
           <t>Armor</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="8" t="inlineStr">
         <is>
           <t>Cargo Capacity (GST)</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="8" t="inlineStr">
         <is>
           <t>Sensor Modifier</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="8" t="inlineStr">
         <is>
           <t>EWDR</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="5" t="inlineStr">
         <is>
           <t>Weapon Systems</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Special Systems</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="5" t="inlineStr">
+        <is>
+          <t>Components</t>
+        </is>
+      </c>
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>Crew Complement</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
+        <is>
+          <t>Rating</t>
+        </is>
+      </c>
+      <c r="P1" s="5" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Falcon Scout</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>300</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>3G/6G/12G</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>8</v>
-      </c>
-      <c r="E2" t="n">
+    <row r="2" ht="135" customHeight="1">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>Vanguard Class - XRV-105</t>
+        </is>
+      </c>
+      <c r="B2" s="9" t="n">
+        <v>1200</v>
+      </c>
+      <c r="C2" s="9" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="9" t="n">
+        <v>12</v>
+      </c>
+      <c r="F2" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="G2" t="n">
-        <v>4</v>
-      </c>
-      <c r="H2" t="n">
-        <v>50</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>+3</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>+2</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Dual Light Pulse Lasers</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Stealth Suite, Advanced Sensor Package</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>3 (Pilot, Sensor Operator, Engineer)</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>The Falcon Scout is a nimble reconnaissance craft designed for rapid deployment and stealth operations. Equipped with advanced sensors and light armament, it excels in gathering intelligence and avoiding detection.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Hawk-Eye Recon</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>280</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3G/5G/10G</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>7</v>
-      </c>
-      <c r="E3" t="n">
-        <v>11</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="H2" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" s="9" t="n">
+        <v>200</v>
+      </c>
+      <c r="J2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="G3" t="n">
-        <v>3</v>
-      </c>
-      <c r="H3" t="n">
-        <v>40</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>+4</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>+1</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Single Gauss Cannon</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Long-Range Scanners, Electronic Countermeasures</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>2 (Pilot, Sensor Operator)</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>The Hawk-Eye Recon is a small, agile scout ship equipped with long-range sensors and minimal armament. Its primary role is to gather intelligence and provide early warning of enemy activity.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Wasp Interceptor</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>350</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>4G/7G/14G</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>9</v>
-      </c>
-      <c r="E4" t="n">
-        <v>9</v>
-      </c>
-      <c r="F4" t="n">
-        <v>7</v>
-      </c>
-      <c r="G4" t="n">
-        <v>5</v>
-      </c>
-      <c r="H4" t="n">
-        <v>60</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>+2</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>+2</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Light Missile Pod, Twin Plasma Cannons</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Enhanced Thrusters, Advanced Targeting System</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>3 (Pilot, Weapons Officer, Engineer)</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>The Wasp Interceptor is a versatile scout craft designed for both reconnaissance and light combat. With its fast acceleration and light weaponry, it can quickly engage and disengage from hostile situations.</t>
+      <c r="L2" s="6" t="inlineStr">
+        <is>
+          <t>['Medium-Range Missile Launchers', 'Point Defense Gauss Weaponry', 'High-Intensity Laser']</t>
+        </is>
+      </c>
+      <c r="M2" s="6" t="inlineStr">
+        <is>
+          <t>['Kramer PAD Drive', 'Small Stellar Projector', 'IRHEC', 'Standard Missile Magazine', 'Advanced Sensors', 'Emergency Repair Systems']</t>
+        </is>
+      </c>
+      <c r="N2" s="9" t="n">
+        <v>45</v>
+      </c>
+      <c r="O2" s="9" t="n">
+        <v>25</v>
+      </c>
+      <c r="P2" s="6" t="inlineStr">
+        <is>
+          <t>The Vanguard Class - XRV-105 is a medium-sized vessel, approximately 45m long, 12m wide, and 10m high. It is designed for multi-role missions, capable of both combat and exploration, including interstellar travel. The ship is equipped with advanced sensor suites, electronic warfare defenses, and a small Stellar Projector powered by an IRHEC, making it suitable for deep space operations. It has moderate cargo capacity, with a well-rounded set of weapons and support systems.</t>
         </is>
       </c>
     </row>
@@ -929,63 +1180,248 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="29.28515625" defaultRowHeight="15"/>
+  <cols>
+    <col width="29.28515625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="24" customWidth="1" style="3" min="2" max="2"/>
+    <col width="29.28515625" customWidth="1" style="3" min="3" max="16384"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="45" customHeight="1">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Component Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Attribute 1</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Attribute 2</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Attribute 3</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Attribute 4</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Weight</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Power Requirement</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Component Size</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Special Properties</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>EWDR</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Rating</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Description</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Attributes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="135" customHeight="1">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>SSP-01</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Small Stellar Projector</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>Allows the ship to perform interstellar jumps within a limited range.</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>The SSP-01 is a compact Stellar Projector designed for medium-sized vessels. It enables interstellar travel within a range of up to 10 lightyears, making it suitable for missions requiring quick hops between nearby star systems. Its high power consumption necessitates robust power management systems.</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>{'Jump Range': 'Up to 10 Lightyears', 'Cooldown Time': '24 hours', 'Power Consumption': 'High'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="180" customHeight="1">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>IRHEC-5</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Power Capacitor</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>Provides the necessary energy burst to power the Stellar Projector for interstellar jumps.</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>The IRHEC-5 is an advanced energy storage system designed to provide a high-energy burst necessary for operating a Stellar Projector. With a capacity of 500 TJ and a recharge time of 6 hours, it ensures that the ship can perform consecutive jumps with minimal downtime.</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>{'Energy Storage Capacity': '500 TJ', 'Recharge Time': '6 hours', 'Output Efficiency': '95%'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="165" customHeight="1">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>AS-12</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Sensor Suite</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>Enhanced sensor resolution for detecting objects and phenomena in deep space.</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>The AS-12 is an advanced sensor suite capable of detecting objects up to 50,000 km away with high resolution. It provides excellent situational awareness in space, especially useful for navigation and threat detection.</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>{'Detection Range': '50,000 km', 'Resolution': 'High', 'Power Consumption': 'Moderate'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="165" customHeight="1">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>KPD-200</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Propulsion System</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Provides propulsion for in-system travel, optimized for long-duration missions.</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>The KPD-200 is a reliable and efficient propulsion system designed for medium-sized vessels. It delivers a maximum acceleration of 4 G and is optimized for fuel efficiency, making it ideal for extended missions within star systems.</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>{'Max Acceleration': '4 G', 'Fuel Efficiency': 'High', 'Power Consumption': 'Moderate'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="150" customHeight="1">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>ERS-3</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Utility System</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>Automated repair system capable of addressing critical damage quickly.</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>The ERS-3 is an automated repair system designed to quickly address critical damage during emergencies. It utilizes advanced robotics to perform repairs with minimal crew intervention, ensuring that the ship remains operational even in the most challenging situations.</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>{'Repair Speed': 'Fast', 'Resource Consumption': 'Moderate', 'Automation Level': 'High'}</t>
         </is>
       </c>
     </row>

</xml_diff>